<commit_message>
Updated for heterogenous date-times; ran 2023 Q1
</commit_message>
<xml_diff>
--- a/output/2022q1-coding-audit.xlsx
+++ b/output/2022q1-coding-audit.xlsx
@@ -4192,8 +4192,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010055E7AF632A704D4CBB1BD9FA14B19970" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c915b622f17d06218f3334f54ec812be">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="edae88a8-d9dc-4074-a55b-fb97cb2cd74d" xmlns:ns3="852f286e-3e14-48be-b416-81218d12f978" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a3db0db921c34a782b6d64d961a8785" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010055E7AF632A704D4CBB1BD9FA14B19970" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5705bc62546c00eb30d3e393ea3d800">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="edae88a8-d9dc-4074-a55b-fb97cb2cd74d" xmlns:ns3="852f286e-3e14-48be-b416-81218d12f978" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c29e53287aa3a112937d5a643cee4298" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="edae88a8-d9dc-4074-a55b-fb97cb2cd74d"/>
     <xsd:import namespace="852f286e-3e14-48be-b416-81218d12f978"/>
@@ -4217,6 +4217,8 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -4295,6 +4297,13 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="23" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c6d7f816-bc26-4675-b66e-019c6d6df9c2" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="852f286e-3e14-48be-b416-81218d12f978" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -4324,6 +4333,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="24" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{470e1751-435f-4e7f-a343-fe3c661a44ef}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="852f286e-3e14-48be-b416-81218d12f978">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -4434,10 +4454,27 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="852f286e-3e14-48be-b416-81218d12f978" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="edae88a8-d9dc-4074-a55b-fb97cb2cd74d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{756DF206-776C-4FE3-A4A8-40D9707D7F98}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C52F50D3-2603-48CE-9D02-539AC37285E9}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{158BB50B-1E87-45DA-997E-E97F481750BD}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2763ADCB-3101-4D61-AE99-50E251FEEC78}"/>
 </file>
</xml_diff>

<commit_message>
Ran August consecutive CPT audit for paths B & D
</commit_message>
<xml_diff>
--- a/output/2022q1-coding-audit.xlsx
+++ b/output/2022q1-coding-audit.xlsx
@@ -4192,8 +4192,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010055E7AF632A704D4CBB1BD9FA14B19970" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5705bc62546c00eb30d3e393ea3d800">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="edae88a8-d9dc-4074-a55b-fb97cb2cd74d" xmlns:ns3="852f286e-3e14-48be-b416-81218d12f978" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c29e53287aa3a112937d5a643cee4298" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010055E7AF632A704D4CBB1BD9FA14B19970" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7a142d422042ab65c5cf1bdc7db96e15">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="edae88a8-d9dc-4074-a55b-fb97cb2cd74d" xmlns:ns3="852f286e-3e14-48be-b416-81218d12f978" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c40a8bb7e01840c9a3629736cac3e4c1" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="edae88a8-d9dc-4074-a55b-fb97cb2cd74d"/>
     <xsd:import namespace="852f286e-3e14-48be-b416-81218d12f978"/>
@@ -4219,6 +4219,7 @@
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -4303,6 +4304,11 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="25" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="852f286e-3e14-48be-b416-81218d12f978" elementFormDefault="qualified">
@@ -4468,7 +4474,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C52F50D3-2603-48CE-9D02-539AC37285E9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31DEC749-D053-4D5B-9627-6EF0FF299031}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>